<commit_message>
Every Time I see! you
</commit_message>
<xml_diff>
--- a/현재인구.xlsx
+++ b/현재인구.xlsx
@@ -1422,8 +1422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29:E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>